<commit_message>
error correction in data set 105
</commit_message>
<xml_diff>
--- a/data/WHO/XLSX files/report 105 - 4 May 2020.xlsx
+++ b/data/WHO/XLSX files/report 105 - 4 May 2020.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lauernd\Desktop\covid data WHO\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lauernd\Documents\R\workspace\COVID-19_epi_info\data\WHO\XLSX files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D542D183-43BB-4D40-9634-7EC7013F5AB2}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDEF9A7C-C3FF-47BD-9D2F-34D5D71B0399}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1275" yWindow="225" windowWidth="15495" windowHeight="9975" xr2:uid="{215388D3-447A-4AA9-8AB9-1870246795A8}"/>
+    <workbookView xWindow="3570" yWindow="-11115" windowWidth="15495" windowHeight="9330" xr2:uid="{215388D3-447A-4AA9-8AB9-1870246795A8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -718,12 +718,6 @@
     <t>Comoros</t>
   </si>
   <si>
-    <t>Curaçao</t>
-  </si>
-  <si>
-    <t>Saint Barthélemy</t>
-  </si>
-  <si>
     <t>Tajikistan</t>
   </si>
   <si>
@@ -739,6 +733,12 @@
       </rPr>
       <t>[1]</t>
     </r>
+  </si>
+  <si>
+    <t>Curacao</t>
+  </si>
+  <si>
+    <t>Saint Barthelemy</t>
   </si>
 </sst>
 </file>
@@ -1135,7 +1135,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B10F8E3E-3B86-4A98-BC35-BE3C4ED8FC3B}">
   <dimension ref="A1:G215"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A86" workbookViewId="0">
+      <selection activeCell="B102" sqref="B102"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3032,7 +3034,7 @@
         <v>92</v>
       </c>
       <c r="B95" s="5" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="C95" s="5">
         <v>16</v>
@@ -3152,7 +3154,7 @@
         <v>92</v>
       </c>
       <c r="B101" s="5" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="C101" s="5">
         <v>6</v>
@@ -4652,7 +4654,7 @@
         <v>7</v>
       </c>
       <c r="B176" s="5" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="C176" s="5">
         <v>128</v>
@@ -4732,7 +4734,7 @@
         <v>89</v>
       </c>
       <c r="B180" s="8" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="C180" s="7">
         <v>851</v>

</xml_diff>